<commit_message>
Corrction of Mouser PN for C4,C32
</commit_message>
<xml_diff>
--- a/05_Docs/BOM FOLDER Ver0.2 12092016.xlsx
+++ b/05_Docs/BOM FOLDER Ver0.2 12092016.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="260">
   <si>
     <t>Qty</t>
   </si>
@@ -799,6 +799,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>81-GRM39C100D50</t>
   </si>
 </sst>
 </file>
@@ -971,7 +974,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1024,17 +1027,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1048,19 +1063,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,14 +1354,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:G2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O48" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="28" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="22" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="17" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" style="17" bestFit="1" customWidth="1"/>
@@ -1365,24 +1371,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
@@ -1408,15 +1414,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
     </row>
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1437,7 +1443,7 @@
       <c r="F5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="23" t="s">
         <v>258</v>
       </c>
     </row>
@@ -2141,15 +2147,15 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
     </row>
     <row r="38" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
@@ -2290,12 +2296,12 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
@@ -2340,8 +2346,8 @@
       <c r="F46" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>215</v>
+      <c r="G46" s="31" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
@@ -2363,7 +2369,7 @@
       <c r="F47" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="G47" s="31" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2529,15 +2535,15 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
     </row>
     <row r="56" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
@@ -2839,15 +2845,15 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="23"/>
-      <c r="E69" s="23"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="23"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="27"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
     </row>
     <row r="70" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
@@ -2873,15 +2879,15 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="24" t="s">
+      <c r="A71" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="28"/>
     </row>
     <row r="72" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
@@ -2907,15 +2913,15 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="25" t="s">
+      <c r="A73" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
     </row>
     <row r="74" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
@@ -2973,13 +2979,13 @@
       <c r="C76" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="D76" s="26" t="s">
+      <c r="D76" s="20" t="s">
         <v>244</v>
       </c>
       <c r="E76" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F76" s="27" t="s">
+      <c r="F76" s="21" t="s">
         <v>243</v>
       </c>
       <c r="G76" s="13" t="s">
@@ -3080,13 +3086,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="A1:G2"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A37:G37"/>
     <mergeCell ref="A55:G55"/>
     <mergeCell ref="A69:G69"/>
     <mergeCell ref="A71:G71"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="A1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>